<commit_message>
corrigido erros na mascara de moedas e adicionado planilha q ensina preço médio
</commit_message>
<xml_diff>
--- a/PLANILHAS/Testando.xlsx
+++ b/PLANILHAS/Testando.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="12108" windowHeight="7560"/>
+    <workbookView windowWidth="21108" windowHeight="13464" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="asdasd" sheetId="1" r:id="rId2"/>
+    <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="27">
   <si>
     <t>Data do Negócio</t>
   </si>
@@ -80,31 +81,63 @@
     <t>(55*1)+(60*5)+(70*1)+(72*2)+(65*10)+(68+5)</t>
   </si>
   <si>
-    <t>1+5+1+2+10+5</t>
-  </si>
-  <si>
     <t>Valor total atual</t>
   </si>
   <si>
     <t>Quantidade total atual</t>
+  </si>
+  <si>
+    <t>Preço Médio</t>
+  </si>
+  <si>
+    <t>Valor Toal</t>
+  </si>
+  <si>
+    <t>CSMG3F</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="180" formatCode="&quot;R$&quot;\ #,##0.00_);[Red]\(&quot;R$&quot;\ #,###.00\)"/>
-    <numFmt numFmtId="181" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="181" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="182" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -525,6 +558,32 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -620,32 +679,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -752,31 +785,19 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -785,235 +806,280 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="180" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="6" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="6" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="181" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="58" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="182" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="58" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1337,408 +1403,408 @@
   <sheetPr/>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="A13" sqref="A13:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.1111111111111" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="31.7777777777778" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6666666666667" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.2222222222222" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5555555555556" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.1111111111111" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.2222222222222" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.2222222222222" style="1" customWidth="1"/>
-    <col min="8" max="16375" width="22.1111111111111" style="1" customWidth="1"/>
-    <col min="16376" max="16384" width="22.1111111111111" style="1"/>
+    <col min="1" max="1" width="31.7777777777778" style="16" customWidth="1"/>
+    <col min="2" max="2" width="16.6666666666667" style="16" customWidth="1"/>
+    <col min="3" max="3" width="20.2222222222222" style="16" customWidth="1"/>
+    <col min="4" max="4" width="19.5555555555556" style="16" customWidth="1"/>
+    <col min="5" max="5" width="22.1111111111111" style="16" customWidth="1"/>
+    <col min="6" max="6" width="15.2222222222222" style="16" customWidth="1"/>
+    <col min="7" max="7" width="14.2222222222222" style="16" customWidth="1"/>
+    <col min="8" max="16375" width="22.1111111111111" style="16" customWidth="1"/>
+    <col min="16376" max="16384" width="22.1111111111111" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="37" customHeight="1" spans="1:9">
-      <c r="A1" s="29" t="s">
+    <row r="1" s="16" customFormat="1" ht="37" customHeight="1" spans="1:9">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="42" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="28.8" spans="1:9">
-      <c r="A2" s="33">
+    <row r="2" s="16" customFormat="1" ht="28.8" spans="1:9">
+      <c r="A2" s="44">
         <v>44958</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="37">
+      <c r="G2" s="48">
         <v>1</v>
       </c>
-      <c r="H2" s="38">
+      <c r="H2" s="49">
         <v>55</v>
       </c>
-      <c r="I2" s="39">
+      <c r="I2" s="50">
         <f t="shared" ref="I2:I13" si="0">H2*G2</f>
         <v>55</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="28.8" spans="1:9">
-      <c r="A3" s="33">
+    <row r="3" s="16" customFormat="1" ht="28.8" spans="1:9">
+      <c r="A3" s="44">
         <v>44961</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="37">
+      <c r="G3" s="48">
         <v>5</v>
       </c>
-      <c r="H3" s="38">
+      <c r="H3" s="49">
         <v>60</v>
       </c>
-      <c r="I3" s="39">
+      <c r="I3" s="50">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="28.8" spans="1:9">
-      <c r="A4" s="33">
+    <row r="4" s="16" customFormat="1" ht="28.8" spans="1:9">
+      <c r="A4" s="44">
         <v>44998</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="F4" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="37">
+      <c r="G4" s="48">
         <v>1</v>
       </c>
-      <c r="H4" s="38">
+      <c r="H4" s="49">
         <v>70</v>
       </c>
-      <c r="I4" s="39">
+      <c r="I4" s="50">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
     </row>
     <row r="5" ht="28.8" spans="1:9">
-      <c r="A5" s="33">
+      <c r="A5" s="44">
         <v>45012</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="37">
+      <c r="G5" s="48">
         <v>2</v>
       </c>
-      <c r="H5" s="38">
+      <c r="H5" s="49">
         <v>72</v>
       </c>
-      <c r="I5" s="39">
+      <c r="I5" s="50">
         <f t="shared" si="0"/>
         <v>144</v>
       </c>
     </row>
     <row r="6" ht="28.8" spans="1:9">
-      <c r="A6" s="33">
+      <c r="A6" s="44">
         <v>45045</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="37">
+      <c r="G6" s="48">
         <v>10</v>
       </c>
-      <c r="H6" s="38">
+      <c r="H6" s="49">
         <v>65</v>
       </c>
-      <c r="I6" s="39">
+      <c r="I6" s="50">
         <f t="shared" si="0"/>
         <v>650</v>
       </c>
     </row>
     <row r="7" ht="28.8" spans="1:9">
-      <c r="A7" s="33">
+      <c r="A7" s="44">
         <v>45056</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="36" t="s">
+      <c r="E7" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="36" t="s">
+      <c r="F7" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="37">
+      <c r="G7" s="48">
         <v>5</v>
       </c>
-      <c r="H7" s="38">
+      <c r="H7" s="49">
         <v>68</v>
       </c>
-      <c r="I7" s="39">
+      <c r="I7" s="50">
         <f t="shared" si="0"/>
         <v>340</v>
       </c>
     </row>
     <row r="8" ht="28.8" spans="1:9">
-      <c r="A8" s="33">
+      <c r="A8" s="44">
         <v>45061</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="37">
+      <c r="G8" s="48">
         <v>3</v>
       </c>
-      <c r="H8" s="38">
+      <c r="H8" s="49">
         <v>70</v>
       </c>
-      <c r="I8" s="39">
+      <c r="I8" s="50">
         <f t="shared" si="0"/>
         <v>210</v>
       </c>
     </row>
     <row r="9" ht="28.8" spans="1:9">
-      <c r="A9" s="33">
+      <c r="A9" s="44">
         <v>45158</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="36" t="s">
+      <c r="E9" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="36" t="s">
+      <c r="F9" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="37">
+      <c r="G9" s="48">
         <v>5</v>
       </c>
-      <c r="H9" s="38">
+      <c r="H9" s="49">
         <v>85</v>
       </c>
-      <c r="I9" s="39">
+      <c r="I9" s="50">
         <f t="shared" si="0"/>
         <v>425</v>
       </c>
     </row>
     <row r="10" ht="28.8" spans="1:9">
-      <c r="A10" s="33">
+      <c r="A10" s="44">
         <v>45196</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="36" t="s">
+      <c r="E10" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="36" t="s">
+      <c r="F10" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="37">
+      <c r="G10" s="48">
         <v>2</v>
       </c>
-      <c r="H10" s="38">
+      <c r="H10" s="49">
         <v>50</v>
       </c>
-      <c r="I10" s="39">
+      <c r="I10" s="50">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
     <row r="11" ht="28.8" spans="1:9">
-      <c r="A11" s="33">
+      <c r="A11" s="44">
         <v>45201</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="36" t="s">
+      <c r="F11" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="37">
+      <c r="G11" s="48">
         <v>10</v>
       </c>
-      <c r="H11" s="38">
+      <c r="H11" s="49">
         <v>70</v>
       </c>
-      <c r="I11" s="39">
+      <c r="I11" s="50">
         <f t="shared" si="0"/>
         <v>700</v>
       </c>
     </row>
     <row r="12" ht="28.8" spans="1:9">
-      <c r="A12" s="33">
+      <c r="A12" s="44">
         <v>45216</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="36" t="s">
+      <c r="E12" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="36" t="s">
+      <c r="F12" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="37">
+      <c r="G12" s="48">
         <v>5</v>
       </c>
-      <c r="H12" s="38">
+      <c r="H12" s="49">
         <v>62</v>
       </c>
-      <c r="I12" s="39">
+      <c r="I12" s="50">
         <f t="shared" si="0"/>
         <v>310</v>
       </c>
     </row>
     <row r="13" ht="28.8" spans="1:9">
-      <c r="A13" s="33">
+      <c r="A13" s="44">
         <v>45255</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="D13" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="36" t="s">
+      <c r="E13" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="36" t="s">
+      <c r="F13" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="37">
+      <c r="G13" s="48">
         <v>18</v>
       </c>
-      <c r="H13" s="38">
+      <c r="H13" s="49">
         <v>64</v>
       </c>
-      <c r="I13" s="39">
+      <c r="I13" s="50">
         <f t="shared" si="0"/>
         <v>1152</v>
       </c>
@@ -1752,527 +1818,653 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B4:P23"/>
+  <dimension ref="B4:P20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7777777777778" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="7.55555555555556" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6666666666667" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7777777777778" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.88888888888889" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.4444444444444" style="1" customWidth="1"/>
-    <col min="6" max="8" width="13.7777777777778" style="1" customWidth="1"/>
-    <col min="9" max="9" width="2.55555555555556" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="13.7777777777778" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.55555555555556" style="16" customWidth="1"/>
+    <col min="2" max="2" width="17.6666666666667" style="16" customWidth="1"/>
+    <col min="3" max="3" width="13.7777777777778" style="16" customWidth="1"/>
+    <col min="4" max="4" width="7.88888888888889" style="16" customWidth="1"/>
+    <col min="5" max="5" width="10.4444444444444" style="16" customWidth="1"/>
+    <col min="6" max="8" width="13.7777777777778" style="16" customWidth="1"/>
+    <col min="9" max="9" width="2.55555555555556" style="16" customWidth="1"/>
+    <col min="10" max="16384" width="13.7777777777778" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" ht="38.4" spans="2:10">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="16" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:12">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="19">
         <v>1</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="20">
         <f>D5</f>
         <v>1</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="21">
         <v>55</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="21">
         <f t="shared" ref="G5:G7" si="0">F5*D5</f>
         <v>55</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="22">
         <f>G5</f>
         <v>55</v>
       </c>
-      <c r="J5" s="20">
+      <c r="J5" s="33">
         <f>F5</f>
         <v>55</v>
       </c>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
     </row>
     <row r="6" spans="2:12">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="24">
         <v>5</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="25">
         <f>D6+E5</f>
         <v>6</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="26">
         <v>60</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="26">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="22">
         <f>G6+H5</f>
         <v>355</v>
       </c>
-      <c r="J6" s="20">
+      <c r="J6" s="33">
         <f>(H6)/(E6)</f>
         <v>59.1666666666667</v>
       </c>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
     </row>
     <row r="7" spans="2:16">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="24">
         <v>1</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="25">
         <f>D7+E6</f>
         <v>7</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="26">
         <v>70</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="26">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="22">
         <f>G7+H6</f>
         <v>425</v>
       </c>
-      <c r="J7" s="20">
+      <c r="J7" s="33">
         <f>(H7)/(E7)</f>
         <v>60.7142857142857</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="K7" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="22"/>
-      <c r="N7" s="20">
+      <c r="L7" s="35"/>
+      <c r="N7" s="33">
         <f>G5+G6+G7+G8+G9+G10</f>
         <v>1559</v>
       </c>
-      <c r="O7" s="1">
+      <c r="O7" s="16">
         <f>D5+D6+D7+D8+D9+D10</f>
         <v>24</v>
       </c>
-      <c r="P7" s="20">
+      <c r="P7" s="33">
         <f>N7/O7</f>
         <v>64.9583333333333</v>
       </c>
     </row>
     <row r="8" spans="2:12">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="24">
         <v>2</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="25">
         <f>D8+E7</f>
         <v>9</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="26">
         <v>72</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="26">
         <f t="shared" ref="G8:G10" si="1">F8*D8</f>
         <v>144</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="22">
         <f>G8+H7</f>
         <v>569</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J8" s="33">
         <f>(H8)/(E8)</f>
         <v>63.2222222222222</v>
       </c>
-      <c r="K8" s="23"/>
-      <c r="L8" s="24"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="37"/>
     </row>
     <row r="9" spans="2:12">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="24">
         <v>10</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="25">
         <f>D9+E8</f>
         <v>19</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="26">
         <v>65</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="26">
         <f t="shared" si="1"/>
         <v>650</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="22">
         <f>G9+H8</f>
         <v>1219</v>
       </c>
-      <c r="J9" s="20">
+      <c r="J9" s="33">
         <f>(H9)/(E9)</f>
         <v>64.1578947368421</v>
       </c>
-      <c r="K9" s="23"/>
-      <c r="L9" s="24"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="37"/>
     </row>
     <row r="10" spans="2:16">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="24">
         <v>5</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="25">
         <f>D10+E9</f>
         <v>24</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="26">
         <v>68</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="26">
         <f t="shared" si="1"/>
         <v>340</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="22">
         <f>G10+H9</f>
         <v>1559</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J10" s="33">
         <f>(H10)/(E10)</f>
         <v>64.9583333333333</v>
       </c>
-      <c r="K10" s="23"/>
-      <c r="L10" s="24"/>
-      <c r="N10" s="25" t="s">
+      <c r="K10" s="36"/>
+      <c r="L10" s="37"/>
+      <c r="N10" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-    </row>
-    <row r="11" spans="2:14">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="7"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="27"/>
-      <c r="N11" s="1" t="s">
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+    </row>
+    <row r="11" spans="2:12">
+      <c r="B11" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="24">
+        <v>3</v>
+      </c>
+      <c r="E11" s="25">
+        <f>E10-D11</f>
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="2:12">
-      <c r="B12" s="8" t="s">
+      <c r="F11" s="26">
+        <v>70</v>
+      </c>
+      <c r="G11" s="26">
+        <f t="shared" ref="G11:G13" si="2">F11*D11</f>
+        <v>210</v>
+      </c>
+      <c r="H11" s="22">
+        <f>IF(B11="Venda",E11*F11,H10+G11)</f>
+        <v>1470</v>
+      </c>
+      <c r="J11" s="33">
+        <f>H11/E11</f>
+        <v>70</v>
+      </c>
+      <c r="K11" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="39"/>
+    </row>
+    <row r="12" spans="2:11">
+      <c r="B12" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="9">
-        <v>3</v>
-      </c>
-      <c r="E12" s="10">
-        <f>E10-D12</f>
-        <v>21</v>
-      </c>
-      <c r="F12" s="11">
-        <v>70</v>
-      </c>
-      <c r="G12" s="11">
-        <f t="shared" ref="G12:G14" si="2">F12*D12</f>
-        <v>210</v>
-      </c>
-      <c r="H12" s="7">
-        <f>H10-G12</f>
-        <v>1349</v>
-      </c>
-      <c r="J12" s="20">
-        <f>H12/E12</f>
-        <v>64.2380952380952</v>
-      </c>
-      <c r="K12" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="L12" s="28"/>
-    </row>
-    <row r="13" spans="2:11">
-      <c r="B13" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="9">
+      <c r="D12" s="24">
         <v>5</v>
       </c>
-      <c r="E13" s="10">
-        <f>E12-D13</f>
+      <c r="E12" s="25">
+        <f>E11-D12</f>
         <v>16</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F12" s="26">
         <v>85</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G12" s="26">
         <f t="shared" si="2"/>
         <v>425</v>
       </c>
-      <c r="H13" s="7">
-        <f>H12-G13</f>
-        <v>924</v>
-      </c>
-      <c r="J13" s="20">
-        <f>H13/E13</f>
-        <v>57.75</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10">
-      <c r="B14" s="8" t="s">
+      <c r="H12" s="22">
+        <f>IF(B12="Venda",E12*F12,H11+G12)</f>
+        <v>1360</v>
+      </c>
+      <c r="J12" s="33">
+        <f>H12/E12</f>
+        <v>85</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C13" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D13" s="24">
         <v>2</v>
       </c>
-      <c r="E14" s="10">
-        <f>E13-D14</f>
+      <c r="E13" s="25">
+        <f>E12-D13</f>
         <v>14</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F13" s="26">
         <v>50</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G13" s="26">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="H14" s="7">
-        <f>H13-G14</f>
-        <v>824</v>
-      </c>
-      <c r="J14" s="20">
+      <c r="H13" s="22">
+        <f>IF(B13="Venda",E13*F13,H12+G13)</f>
+        <v>700</v>
+      </c>
+      <c r="J13" s="33">
+        <f>H13/E13</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14">
+      <c r="B14" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="24">
+        <v>10</v>
+      </c>
+      <c r="E14" s="25">
+        <f>E13+D14</f>
+        <v>24</v>
+      </c>
+      <c r="F14" s="26">
+        <v>70</v>
+      </c>
+      <c r="G14" s="26">
+        <f>F14*D14</f>
+        <v>700</v>
+      </c>
+      <c r="H14" s="22">
+        <f>IF(B14="Venda",E14*F14,H13+G14)</f>
+        <v>1400</v>
+      </c>
+      <c r="J14" s="33">
         <f>H14/E14</f>
-        <v>58.8571428571429</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14">
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="16"/>
-      <c r="N15" s="20"/>
-    </row>
-    <row r="16" spans="2:14">
-      <c r="B16" s="8" t="s">
+        <v>58.3333333333333</v>
+      </c>
+      <c r="N14" s="33"/>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C15" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="9">
-        <v>10</v>
-      </c>
-      <c r="E16" s="10">
-        <f>E14+D16</f>
-        <v>24</v>
-      </c>
-      <c r="F16" s="11">
-        <v>70</v>
-      </c>
-      <c r="G16" s="11">
-        <f t="shared" ref="G16:G19" si="3">F16*D16</f>
-        <v>700</v>
-      </c>
-      <c r="H16" s="7">
-        <f>H14+G16</f>
-        <v>1524</v>
-      </c>
-      <c r="J16" s="20">
+      <c r="D15" s="24">
+        <v>5</v>
+      </c>
+      <c r="E15" s="25">
+        <f>E14+D15</f>
+        <v>29</v>
+      </c>
+      <c r="F15" s="26">
+        <v>62</v>
+      </c>
+      <c r="G15" s="26">
+        <f>F15*D15</f>
+        <v>310</v>
+      </c>
+      <c r="H15" s="22">
+        <f>IF(B15="Venda",E15*F15,H14+G15)</f>
+        <v>1710</v>
+      </c>
+      <c r="J15" s="33">
+        <f>H15/E15</f>
+        <v>58.9655172413793</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="24">
+        <v>18</v>
+      </c>
+      <c r="E16" s="25">
+        <f>E15-D16</f>
+        <v>11</v>
+      </c>
+      <c r="F16" s="26">
+        <v>64</v>
+      </c>
+      <c r="G16" s="26">
+        <f>F16*D16</f>
+        <v>1152</v>
+      </c>
+      <c r="H16" s="22">
+        <f>IF(B16="Venda",E16*F16,H15+G16)</f>
+        <v>704</v>
+      </c>
+      <c r="J16" s="33">
         <f>H16/E16</f>
-        <v>63.5</v>
-      </c>
-      <c r="N16" s="20"/>
-    </row>
-    <row r="17" spans="2:10">
-      <c r="B17" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="9">
-        <v>5</v>
-      </c>
-      <c r="E17" s="10">
-        <f>E16+D17</f>
-        <v>29</v>
-      </c>
-      <c r="F17" s="11">
-        <v>62</v>
-      </c>
-      <c r="G17" s="11">
-        <f t="shared" si="3"/>
-        <v>310</v>
-      </c>
-      <c r="H17" s="7">
-        <f>H16+G17</f>
-        <v>1834</v>
-      </c>
-      <c r="J17" s="20">
-        <f>H17/E17</f>
-        <v>63.2413793103448</v>
-      </c>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="28"/>
     </row>
     <row r="18" spans="2:8">
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="13"/>
-    </row>
-    <row r="19" spans="2:10">
-      <c r="B19" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="9">
-        <v>18</v>
-      </c>
-      <c r="E19" s="10">
-        <f>E17-D19</f>
-        <v>11</v>
-      </c>
-      <c r="F19" s="11">
-        <v>64</v>
-      </c>
-      <c r="G19" s="11">
-        <f>F19*D19</f>
-        <v>1152</v>
-      </c>
-      <c r="H19" s="7">
-        <f>H17-G19</f>
-        <v>682</v>
-      </c>
-      <c r="J19" s="20">
-        <f>H19/E19</f>
-        <v>62</v>
-      </c>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="28"/>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="28"/>
     </row>
     <row r="20" spans="2:8">
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="13"/>
-    </row>
-    <row r="21" spans="2:8">
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="13"/>
-    </row>
-    <row r="22" spans="2:8">
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="13"/>
-    </row>
-    <row r="23" spans="2:8">
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="18"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="N10:P10"/>
-    <mergeCell ref="N11:P11"/>
+    <mergeCell ref="K11:L11"/>
     <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K7:L11"/>
+    <mergeCell ref="K7:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="C4:J17"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="3" width="8.88888888888889" style="2"/>
+    <col min="4" max="4" width="11.5555555555556" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.8888888888889" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.4444444444444" style="3" customWidth="1"/>
+    <col min="7" max="7" width="16.2222222222222" style="3" customWidth="1"/>
+    <col min="8" max="9" width="8.88888888888889" style="2"/>
+    <col min="10" max="10" width="12.7777777777778" style="2"/>
+    <col min="11" max="16384" width="8.88888888888889" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:7">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7">
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7">
+        <v>10</v>
+      </c>
+      <c r="F5" s="8">
+        <f>G5/E5</f>
+        <v>10</v>
+      </c>
+      <c r="G5" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7">
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="3:10">
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="J7" s="3">
+        <f>((E5*F5)+(E11*F11))/(E5+E11)</f>
+        <v>-17.88</v>
+      </c>
+    </row>
+    <row r="8" s="1" customFormat="1" ht="26" customHeight="1" spans="3:7">
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+    </row>
+    <row r="9" spans="3:7">
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="3:7">
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="3:7">
+      <c r="C11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="11">
+        <v>-8</v>
+      </c>
+      <c r="F11" s="12">
+        <v>16.97</v>
+      </c>
+      <c r="G11" s="12">
+        <f>E11*F11</f>
+        <v>-135.76</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7">
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="3:7">
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="3:7">
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="3:7">
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="17" spans="3:7">
+      <c r="C17" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="15">
+        <f>SUM(E5:E15)</f>
+        <v>2</v>
+      </c>
+      <c r="F17" s="8">
+        <f>F5</f>
+        <v>10</v>
+      </c>
+      <c r="G17" s="8">
+        <f>F17*E17</f>
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C17:D17"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>